<commit_message>
Date: 03 Nov 2025
</commit_message>
<xml_diff>
--- a/SeleniumAutomationProject/ExcelFile/OHRM_LoginData.xlsx
+++ b/SeleniumAutomationProject/ExcelFile/OHRM_LoginData.xlsx
@@ -39,6 +39,9 @@
     <t>Not Run</t>
   </si>
   <si>
+    <t>rohini</t>
+  </si>
+  <si>
     <t>rohini123</t>
   </si>
   <si>
@@ -60,13 +63,10 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>ragini</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>vbnvn vbn</t>
+    <t>manda user</t>
   </si>
   <si>
     <t>Fail</t>
@@ -80,13 +80,43 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+      <color indexed="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,8 +139,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +429,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -420,7 +455,7 @@
       <c r="B2" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s" s="1">
         <v>14</v>
       </c>
       <c r="D2" t="s" s="0">
@@ -429,12 +464,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="0">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="2">
         <v>16</v>
       </c>
       <c r="D3" t="s" s="0">
@@ -448,7 +483,7 @@
       <c r="B4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s" s="3">
         <v>14</v>
       </c>
       <c r="D4" t="s" s="0">
@@ -457,12 +492,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s" s="4">
         <v>16</v>
       </c>
       <c r="D5" t="s" s="0">
@@ -471,12 +506,12 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="5">
         <v>16</v>
       </c>
       <c r="D6" t="s" s="0">

</xml_diff>